<commit_message>
Finished the 26650 firotch data and add some plot
</commit_message>
<xml_diff>
--- a/data/internal resistance/26650F_IR.xlsx
+++ b/data/internal resistance/26650F_IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Desktop\Battery_lowtemperature\pythonProject\data\internal resistance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA80CB8B-48ED-46C8-B83A-FFCE6074F220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706975C6-7E48-47F3-AD1F-E3FCA39E714C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,7 +377,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,9 +532,24 @@
       <c r="A7">
         <v>-30</v>
       </c>
-      <c r="G7" t="e">
+      <c r="B7">
+        <v>8279</v>
+      </c>
+      <c r="C7">
+        <v>3.9854799999999999</v>
+      </c>
+      <c r="D7">
+        <v>3.1343200000000002</v>
+      </c>
+      <c r="E7">
+        <v>-1.0399999999999999E-3</v>
+      </c>
+      <c r="F7">
+        <v>-4.4966699999999999</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.18933052764573588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>